<commit_message>
added global & local share variable files and mass update to apply global & local variables.
</commit_message>
<xml_diff>
--- a/SystemTest/SystemTestExecutionResult_LPH_V1.9.3.xlsx
+++ b/SystemTest/SystemTestExecutionResult_LPH_V1.9.3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20865" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="21930" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="132">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -412,6 +412,9 @@
   </si>
   <si>
     <t>Copy of Items feature is onHold in LPH</t>
+  </si>
+  <si>
+    <t>Script need more time to fix the maintenance issue.</t>
   </si>
 </sst>
 </file>
@@ -807,7 +810,7 @@
   <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1192,9 +1195,13 @@
       <c r="E17" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F17" s="5"/>
+      <c r="F17" s="9" t="s">
+        <v>129</v>
+      </c>
       <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
+      <c r="H17" s="5" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
@@ -1232,7 +1239,9 @@
       <c r="E19" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F19" s="5"/>
+      <c r="F19" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
     </row>

</xml_diff>